<commit_message>
time remove if 0
</commit_message>
<xml_diff>
--- a/public/demo_sheet.xlsx
+++ b/public/demo_sheet.xlsx
@@ -3809,47 +3809,56 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF999999"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -12488,7 +12497,9 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12526,9 +12537,7 @@
       <c r="C2" s="16">
         <v>44014</v>
       </c>
-      <c r="D2" s="17">
-        <v>0.83333333333333337</v>
-      </c>
+      <c r="D2" s="17"/>
       <c r="E2" s="18" t="s">
         <v>1196</v>
       </c>

</xml_diff>